<commit_message>
Fix mistakes in comments
</commit_message>
<xml_diff>
--- a/Parametric/Param_2.xlsx
+++ b/Parametric/Param_2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Test: bpu_2 (Parameter = 2)</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">saturating_two_bits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main loop is always taken and predictor knows it after the first time =&gt; 1/3 predictions is true. Tested branch is jump from for and has two stages: t0 = 1 – jump, t0 = 0 – not jump. =&gt; WEAKLY NT becomes WEAKLY T after 1, but WEAKLY T becomes WEAKLY NT after 0. It changes after each prediction  and it always fail =&gt; 2/3 of all predictions is fail. 66.67%(it isn’t better then one bit, because we can’t use strongly NT and T)</t>
   </si>
   <si>
     <t xml:space="preserve">adaptive_two_levels</t>
@@ -90,6 +87,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,7 +159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,7 +167,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,7 +199,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -310,13 +309,13 @@
         <v>0.666667</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>1E-005</v>
@@ -325,7 +324,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>